<commit_message>
fix computer science only filter
</commit_message>
<xml_diff>
--- a/profile_author/Lorenzo Stacchio.xlsx
+++ b/profile_author/Lorenzo Stacchio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -962,7 +962,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Flying in XR: Bridging Desktop Applications in eXtended Reality through Deep Learning</t>
+          <t>Fashion in the Metaverse: Technologies, Applications, and Opportunities</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -972,13 +972,13 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>IEEE Conference on Virtual Reality and 3D User Interfaces Abstracts and Workshops (VRW) (pp. 264-272)</t>
+          <t>International Conference on Entertainment Computing</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
@@ -988,7 +988,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>WiXaRd: Towards a holistic distributed platform for multi-party and cross-reality WebXR experiences</t>
+          <t>Social cognition and Metaverse: understanding and disposition towards Human Digital Twins</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -998,13 +998,13 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>IEEE Conference on Virtual Reality and 3D User Interfaces Abstracts and Workshops (VRW).</t>
+          <t>Atti del Congresso dell'Associazione Italiana di Psicologia 2022</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2022</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>M-AGEW: Empowering Outdoor Workouts with Data-Driven Augmented Reality Assistance</t>
+          <t>Flying in XR: Bridging Desktop Applications in eXtended Reality through Deep Learning</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024 IEEE International Conference on Artificial Intelligence and eXtended and Virtual Reality (AIxVR)</t>
+          <t>IEEE Conference on Virtual Reality and 3D User Interfaces Abstracts and Workshops (VRW) (pp. 264-272)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1040,25 +1040,129 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>WiXaRd: Towards a holistic distributed platform for multi-party and cross-reality WebXR experiences</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>inproceedings</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>IEEE Conference on Virtual Reality and 3D User Interfaces Abstracts and Workshops (VRW).</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>M-AGEW: Empowering Outdoor Workouts with Data-Driven Augmented Reality Assistance</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>inproceedings</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2024 IEEE International Conference on Artificial Intelligence and eXtended and Virtual Reality (AIxVR)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AI for Enhancing and Preserving Dance Cultural Heritage: a Case Study on Rudolf Nureyev's Costumes</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>inproceedings</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>The First International Conference on Artificial Intelligence and Immersive Virtual Reality - AIVR 2024</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>DanXe: An extended artificial intelligence framework to analyze and promote dance heritage</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>article</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Digital Applications in Archaeology and Cultural Heritage</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>Q2</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>An Ethical Framework for Trustworthy Neural Rendering applied in Cultural Heritage and Creative Industries</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>inproceedings</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CVPR 2024, AI for 3D Generation Workshop</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
         <is>
           <t>2024</t>
         </is>

</xml_diff>